<commit_message>
Archivos Guion 04 grado 03
Guion con comentarios para autor
</commit_message>
<xml_diff>
--- a/seguimiento/Grado03.xlsx
+++ b/seguimiento/Grado03.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10830" windowHeight="2865"/>
@@ -10,8 +10,8 @@
     <sheet name="Seguimiento" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Editorial</t>
   </si>
@@ -61,13 +61,16 @@
   </si>
   <si>
     <t>Ciencias Naturales</t>
+  </si>
+  <si>
+    <t>En revisión por parte de editor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -423,11 +426,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -545,6 +561,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,21 +837,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
     <col min="2" max="5" width="11.140625" style="1" customWidth="1"/>
@@ -846,7 +865,7 @@
     <col min="13" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickBot="1">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="27" t="s">
         <v>11</v>
       </c>
@@ -855,21 +874,21 @@
       </c>
       <c r="D1" s="33"/>
     </row>
-    <row r="2" spans="1:12" ht="16.5" thickBot="1">
+    <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="34">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="1:12" ht="16.5" thickBot="1">
+    <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="16.5" thickBot="1">
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
@@ -893,7 +912,7 @@
       </c>
       <c r="L4" s="31"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="30.75" thickBot="1">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36"/>
       <c r="B5" s="22" t="s">
         <v>2</v>
@@ -929,7 +948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16.5" thickBot="1">
+    <row r="6" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>1</v>
       </c>
@@ -945,7 +964,7 @@
       <c r="K6" s="14"/>
       <c r="L6" s="15"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5" thickBot="1">
+    <row r="7" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>2</v>
       </c>
@@ -961,7 +980,7 @@
       <c r="K7" s="14"/>
       <c r="L7" s="15"/>
     </row>
-    <row r="8" spans="1:12" ht="16.5" thickBot="1">
+    <row r="8" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29">
         <v>3</v>
       </c>
@@ -977,15 +996,25 @@
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:12" ht="16.5" thickBot="1">
+    <row r="9" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>4</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="40">
+        <v>42075</v>
+      </c>
+      <c r="C9" s="5">
+        <v>42075</v>
+      </c>
+      <c r="D9" s="5">
+        <v>42075</v>
+      </c>
+      <c r="E9" s="5">
+        <v>42075</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="G9" s="10"/>
       <c r="H9" s="11"/>
       <c r="I9" s="18"/>
@@ -993,7 +1022,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:12" ht="16.5" thickBot="1">
+    <row r="10" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>5</v>
       </c>
@@ -1009,7 +1038,7 @@
       <c r="K10" s="14"/>
       <c r="L10" s="15"/>
     </row>
-    <row r="11" spans="1:12" ht="16.5" thickBot="1">
+    <row r="11" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>6</v>
       </c>
@@ -1025,7 +1054,7 @@
       <c r="K11" s="14"/>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="1:12" ht="16.5" thickBot="1">
+    <row r="12" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>7</v>
       </c>
@@ -1049,7 +1078,7 @@
       <c r="K12" s="14"/>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5" thickBot="1">
+    <row r="13" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>8</v>
       </c>
@@ -1065,7 +1094,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:12" ht="16.5" thickBot="1">
+    <row r="14" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>9</v>
       </c>
@@ -1081,7 +1110,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5" thickBot="1">
+    <row r="15" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>10</v>
       </c>
@@ -1097,7 +1126,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="15"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5" thickBot="1">
+    <row r="16" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29">
         <v>11</v>
       </c>
@@ -1113,7 +1142,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="15"/>
     </row>
-    <row r="17" spans="1:12" ht="16.5" thickBot="1">
+    <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29">
         <v>12</v>
       </c>
@@ -1129,7 +1158,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="15"/>
     </row>
-    <row r="18" spans="1:12" ht="16.5" thickBot="1">
+    <row r="18" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>13</v>
       </c>
@@ -1153,7 +1182,7 @@
       <c r="K18" s="14"/>
       <c r="L18" s="15"/>
     </row>
-    <row r="19" spans="1:12" ht="16.5" thickBot="1">
+    <row r="19" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29">
         <v>14</v>
       </c>
@@ -1169,7 +1198,7 @@
       <c r="K19" s="14"/>
       <c r="L19" s="15"/>
     </row>
-    <row r="20" spans="1:12" ht="16.5" thickBot="1">
+    <row r="20" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29">
         <v>15</v>
       </c>
@@ -1185,7 +1214,7 @@
       <c r="K20" s="14"/>
       <c r="L20" s="15"/>
     </row>
-    <row r="21" spans="1:12" ht="16.5" thickBot="1">
+    <row r="21" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Inicio lectura de coordinadora
</commit_message>
<xml_diff>
--- a/seguimiento/Grado03.xlsx
+++ b/seguimiento/Grado03.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Desktop\CienciasNaturales\seguimiento\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10830" windowHeight="2865"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Editorial</t>
   </si>
@@ -64,6 +69,9 @@
   </si>
   <si>
     <t>En revisión por parte de editor</t>
+  </si>
+  <si>
+    <t>En manuscrito de autor</t>
   </si>
 </sst>
 </file>
@@ -837,7 +845,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -847,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +964,9 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
       <c r="I6" s="18"/>
@@ -972,7 +982,9 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
       <c r="I7" s="18"/>
@@ -1058,18 +1070,10 @@
       <c r="A12" s="29">
         <v>7</v>
       </c>
-      <c r="B12" s="4">
-        <v>42080</v>
-      </c>
-      <c r="C12" s="4">
-        <v>42080</v>
-      </c>
-      <c r="D12" s="4">
-        <v>42080</v>
-      </c>
-      <c r="E12" s="4">
-        <v>42080</v>
-      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="6"/>
       <c r="G12" s="10"/>
       <c r="H12" s="11"/>

</xml_diff>

<commit_message>
Notas de seguimiento día 05-04-2015
</commit_message>
<xml_diff>
--- a/seguimiento/Grado03.xlsx
+++ b/seguimiento/Grado03.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Desktop\CienciasNaturales\seguimiento\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10830" windowHeight="2865"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Editorial</t>
   </si>
@@ -68,10 +63,10 @@
     <t>Ciencias Naturales</t>
   </si>
   <si>
-    <t>En revisión por parte de editor</t>
-  </si>
-  <si>
-    <t>En manuscrito de autor</t>
+    <t>En revisión de editor</t>
+  </si>
+  <si>
+    <t>Cuaderno de estudio</t>
   </si>
 </sst>
 </file>
@@ -845,7 +840,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -856,7 +851,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1003,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>4</v>
       </c>
@@ -1042,7 +1037,9 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="G10" s="10"/>
       <c r="H10" s="11"/>
       <c r="I10" s="18"/>

</xml_diff>

<commit_message>
Actualización revisión CN 03 05
Actualización revisión CN 03 05   y formato seguimiento
</commit_message>
<xml_diff>
--- a/seguimiento/Grado03.xlsx
+++ b/seguimiento/Grado03.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Editorial</t>
   </si>
@@ -63,10 +63,13 @@
     <t>Ciencias Naturales</t>
   </si>
   <si>
-    <t>En revisión de editor</t>
-  </si>
-  <si>
-    <t>Cuaderno de estudio</t>
+    <t>Revisado - Pnte cambio motores M</t>
+  </si>
+  <si>
+    <t>En Revisión</t>
+  </si>
+  <si>
+    <t>En revisión</t>
   </si>
 </sst>
 </file>
@@ -840,7 +843,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -850,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,12 +958,14 @@
       <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4">
+        <v>42110</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
@@ -977,9 +982,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
       <c r="I7" s="18"/>
@@ -1003,7 +1006,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>4</v>
       </c>
@@ -1033,12 +1036,16 @@
       <c r="A10" s="29">
         <v>5</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="4">
+        <v>42107</v>
+      </c>
+      <c r="C10" s="4">
+        <v>42107</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="11"/>

</xml_diff>